<commit_message>
Fixed percentage in summary
</commit_message>
<xml_diff>
--- a/Questionaire_calculations.xlsx
+++ b/Questionaire_calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Downloads\SDI grp project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CE158B6-F86C-43B1-A340-99BDB9B26474}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E9C7EC9-EE5E-4897-B2EF-F9905DB7DD2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D1657234-94E6-4BED-AE50-AA4F8CA92BC5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{D1657234-94E6-4BED-AE50-AA4F8CA92BC5}"/>
   </bookViews>
   <sheets>
     <sheet name="Initial Response Calc" sheetId="1" r:id="rId1"/>
@@ -776,8 +776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{166A0867-15D9-4593-B242-8DC1D9D60185}">
   <dimension ref="A1:S34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="P29" sqref="P29"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19:E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1977,8 +1977,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D0870BA-078B-4F2B-8B07-53FA106A9047}">
   <dimension ref="A1:N51"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="Q50" sqref="Q50"/>
+    <sheetView topLeftCell="C20" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:K44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4309,8 +4309,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F882926E-D2F5-4F2C-8190-394716CD5512}">
   <dimension ref="A1:N46"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="N42" sqref="N42"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:K39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6402,10 +6402,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9678449B-4CE6-4251-9EDA-934998063DC1}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6438,8 +6438,8 @@
         <v>43</v>
       </c>
       <c r="C2" s="13">
-        <f>(D2/(D2+D3))*100</f>
-        <v>47.147895503790835</v>
+        <f>(B2/(B2+B3))*100</f>
+        <v>53.086419753086425</v>
       </c>
       <c r="D2" s="13">
         <v>27.325581395348838</v>
@@ -6456,8 +6456,8 @@
         <v>38</v>
       </c>
       <c r="C3" s="13">
-        <f>(D3/(D2+D3))*100</f>
-        <v>52.852104496209165</v>
+        <f>(B3/(B3+B2))*100</f>
+        <v>46.913580246913575</v>
       </c>
       <c r="D3" s="13">
         <v>30.631578947368421</v>
@@ -6466,8 +6466,14 @@
         <v>3.74</v>
       </c>
     </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C4" s="8"/>
+    </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C5" s="8"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C6" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>